<commit_message>
Initial commit with source code.
</commit_message>
<xml_diff>
--- a/BordxGenerator/Reports/20160801-20170630.xlsx
+++ b/BordxGenerator/Reports/20160801-20170630.xlsx
@@ -9,6 +9,7 @@
   <x:sheets>
     <x:sheet name="2016-10" sheetId="191" r:id="rId1"/>
     <x:sheet name="2016-11" sheetId="6" r:id="rId6"/>
+    <x:sheet name="2017-10" sheetId="7" r:id="rId7"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2016-10'!$A$9:$AX$9</x:definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="319">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="375">
   <x:si>
     <x:t>Claims Bordereaux</x:t>
   </x:si>
@@ -978,13 +979,181 @@
   </x:si>
   <x:si>
     <x:t>Multiplan (Check #: 2442)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8/1/2016 - 6/30/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Beker Marisa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>202594-17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5/24/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5/25/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0002659/1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>G45.9-Transient cerebral ischemic attack, unspecified</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/19/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6/6/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0002661/1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C34.92-Malignant neoplasm of unsp part of left bronchus or lung (Malignant neoplasm of unspecified part of left bronchus or lung)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>De`Gasparis Maishka</x:t>
+  </x:si>
+  <x:si>
+    <x:t>De`Gasparis Humberto</x:t>
+  </x:si>
+  <x:si>
+    <x:t>202624-17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3/23/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3/31/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0002642/2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Z90.710-hysterectomy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5620 Lakeshore Dr.Columbia, SC  29206</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/24/2016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001374/13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4/8/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001620/5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/12/2016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001620/6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Van-Dam Lila</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4/4/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5/1/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001619/8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001619/9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3/24/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0002129/4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Van-Dam  Tali</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Van-Dam Mauricio</x:t>
+  </x:si>
+  <x:si>
+    <x:t>202692-17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4/21/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001642/7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>V20.2-Well child check</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Van-Dam  Tamar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001728/6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Benjamín Van-Dam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4/20/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001853/10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Van-Dam Arie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6/16/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6/23/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0002330/7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5/8/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0002415/2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>R53.83-Other fatigue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5/17/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10/25/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Beracha Alan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2/14/2017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L0001550/5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2/16/2017</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:numFmts count="13">
+  <x:numFmts count="27">
     <x:numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <x:numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <x:numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -998,8 +1167,22 @@
     <x:numFmt numFmtId="10" formatCode=""/>
     <x:numFmt numFmtId="11" formatCode=""/>
     <x:numFmt numFmtId="12" formatCode=""/>
+    <x:numFmt numFmtId="13" formatCode=""/>
+    <x:numFmt numFmtId="14" formatCode=""/>
+    <x:numFmt numFmtId="15" formatCode=""/>
+    <x:numFmt numFmtId="16" formatCode=""/>
+    <x:numFmt numFmtId="17" formatCode=""/>
+    <x:numFmt numFmtId="18" formatCode=""/>
+    <x:numFmt numFmtId="19" formatCode=""/>
+    <x:numFmt numFmtId="20" formatCode=""/>
+    <x:numFmt numFmtId="21" formatCode=""/>
+    <x:numFmt numFmtId="22" formatCode=""/>
+    <x:numFmt numFmtId="23" formatCode=""/>
+    <x:numFmt numFmtId="24" formatCode=""/>
+    <x:numFmt numFmtId="25" formatCode=""/>
+    <x:numFmt numFmtId="26" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="19" x14ac:knownFonts="1">
+  <x:fonts count="33" x14ac:knownFonts="1">
     <x:font>
       <x:sz val="10"/>
       <x:name val="Arial"/>
@@ -1056,6 +1239,104 @@
     <x:font>
       <x:sz val="12"/>
       <x:color rgb="FF003082"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
@@ -1234,7 +1515,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="150">
+  <x:cellStyleXfs count="374">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <x:xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1373,6 +1654,678 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="6" fontId="2" fillId="5" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="4" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -11665,4 +12618,2215 @@
   </x:headerFooter>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:BD9"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="12.75"/>
+  <x:cols>
+    <x:col min="1" max="1" width="32.42578125" style="27" customWidth="1"/>
+    <x:col min="2" max="2" width="32.5703125" style="27" customWidth="1"/>
+    <x:col min="3" max="3" width="13.85546875" style="27" customWidth="1"/>
+    <x:col min="4" max="4" width="31.42578125" style="27" customWidth="1"/>
+    <x:col min="5" max="5" width="61.5703125" style="27" customWidth="1"/>
+    <x:col min="6" max="6" width="22.140625" style="27" customWidth="1"/>
+    <x:col min="7" max="9" width="12.85546875" style="27" customWidth="1"/>
+    <x:col min="10" max="11" width="11.5703125" style="27" customWidth="1"/>
+    <x:col min="12" max="12" width="9.5703125" style="27" customWidth="1"/>
+    <x:col min="13" max="15" width="11.42578125" style="27" customWidth="1"/>
+    <x:col min="16" max="16" width="13.140625" style="27" customWidth="1"/>
+    <x:col min="17" max="17" width="10.140625" style="27" customWidth="1"/>
+    <x:col min="18" max="18" width="9.5703125" style="27" customWidth="1"/>
+    <x:col min="19" max="21" width="11.5703125" style="27" customWidth="1"/>
+    <x:col min="22" max="22" width="49.85546875" style="27" customWidth="1"/>
+    <x:col min="23" max="25" width="15.5703125" style="27" customWidth="1"/>
+    <x:col min="26" max="26" width="16.42578125" style="27" customWidth="1"/>
+    <x:col min="27" max="27" width="14.42578125" style="27" customWidth="1"/>
+    <x:col min="28" max="30" width="15.5703125" style="27" customWidth="1"/>
+    <x:col min="31" max="31" width="10.5703125" style="27" customWidth="1"/>
+    <x:col min="32" max="32" width="14.42578125" style="27" customWidth="1"/>
+    <x:col min="33" max="33" width="14.5703125" style="27" customWidth="1"/>
+    <x:col min="34" max="34" width="15.5703125" style="27" customWidth="1"/>
+    <x:col min="35" max="35" width="18.42578125" style="27" customWidth="1"/>
+    <x:col min="36" max="36" width="10.42578125" style="27" customWidth="1"/>
+    <x:col min="37" max="49" width="13.5703125" style="27" customWidth="1"/>
+    <x:col min="50" max="50" width="9.140625" style="27" customWidth="1"/>
+    <x:col min="51" max="51" width="10.42578125" style="27" customWidth="1"/>
+    <x:col min="52" max="54" width="11.5703125" style="27" customWidth="1"/>
+    <x:col min="55" max="55" width="8.42578125" style="27" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:56" customFormat="1" ht="24" customHeight="1">
+      <x:c r="A1" s="28" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="29" t="s"/>
+      <x:c r="C1" s="29" t="s"/>
+      <x:c r="D1" s="29" t="s"/>
+      <x:c r="E1" s="29" t="s"/>
+      <x:c r="F1" s="29" t="s"/>
+      <x:c r="G1" s="27" t="s"/>
+      <x:c r="H1" s="27" t="s"/>
+      <x:c r="I1" s="27" t="s"/>
+      <x:c r="J1" s="27" t="s"/>
+      <x:c r="K1" s="27" t="s"/>
+      <x:c r="L1" s="27" t="s"/>
+      <x:c r="M1" s="27" t="s"/>
+      <x:c r="N1" s="27" t="s"/>
+      <x:c r="O1" s="27" t="s"/>
+      <x:c r="P1" s="27" t="s"/>
+      <x:c r="Q1" s="27" t="s"/>
+      <x:c r="R1" s="27" t="s"/>
+      <x:c r="S1" s="27" t="s"/>
+      <x:c r="T1" s="27" t="s"/>
+      <x:c r="U1" s="27" t="s"/>
+      <x:c r="V1" s="27" t="s"/>
+      <x:c r="W1" s="27" t="s"/>
+      <x:c r="X1" s="27" t="s"/>
+      <x:c r="Y1" s="27" t="s"/>
+      <x:c r="Z1" s="27" t="s"/>
+      <x:c r="AA1" s="27" t="s"/>
+      <x:c r="AB1" s="30" t="s"/>
+      <x:c r="AC1" s="30" t="s"/>
+      <x:c r="AD1" s="30" t="s"/>
+      <x:c r="AE1" s="30" t="s"/>
+      <x:c r="AF1" s="30" t="s"/>
+      <x:c r="AG1" s="30" t="s"/>
+      <x:c r="AH1" s="30" t="s"/>
+      <x:c r="AI1" s="30" t="s"/>
+      <x:c r="AJ1" s="30" t="s"/>
+      <x:c r="AK1" s="30" t="s"/>
+      <x:c r="AL1" s="30" t="s"/>
+      <x:c r="AM1" s="30" t="s"/>
+      <x:c r="AN1" s="31" t="s"/>
+      <x:c r="AO1" s="30" t="s"/>
+      <x:c r="AP1" s="30" t="s"/>
+      <x:c r="AQ1" s="30" t="s"/>
+      <x:c r="AR1" s="30" t="s"/>
+      <x:c r="AS1" s="30" t="s"/>
+      <x:c r="AT1" s="30" t="s"/>
+      <x:c r="AU1" s="30" t="s"/>
+      <x:c r="AV1" s="30" t="s"/>
+      <x:c r="AW1" s="30" t="s"/>
+      <x:c r="AX1" s="30" t="s"/>
+      <x:c r="AY1" s="27" t="s"/>
+      <x:c r="AZ1" s="27" t="s"/>
+      <x:c r="BA1" s="27" t="s"/>
+      <x:c r="BB1" s="27" t="s"/>
+      <x:c r="BC1" s="27" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:56" customFormat="1" ht="18.75" customHeight="1">
+      <x:c r="A2" s="32" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B2" s="27" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C2" s="33" t="s"/>
+      <x:c r="D2" s="33" t="s"/>
+      <x:c r="E2" s="33" t="s"/>
+      <x:c r="F2" s="33" t="s"/>
+      <x:c r="G2" s="27" t="s"/>
+      <x:c r="H2" s="27" t="s"/>
+      <x:c r="I2" s="27" t="s"/>
+      <x:c r="J2" s="27" t="s"/>
+      <x:c r="K2" s="27" t="s"/>
+      <x:c r="L2" s="27" t="s"/>
+      <x:c r="M2" s="27" t="s"/>
+      <x:c r="N2" s="27" t="s"/>
+      <x:c r="O2" s="27" t="s"/>
+      <x:c r="P2" s="27" t="s"/>
+      <x:c r="Q2" s="27" t="s"/>
+      <x:c r="R2" s="27" t="s"/>
+      <x:c r="S2" s="27" t="s"/>
+      <x:c r="T2" s="27" t="s"/>
+      <x:c r="U2" s="27" t="s"/>
+      <x:c r="V2" s="27" t="s"/>
+      <x:c r="W2" s="27" t="s"/>
+      <x:c r="X2" s="27" t="s"/>
+      <x:c r="Y2" s="27" t="s"/>
+      <x:c r="Z2" s="27" t="s"/>
+      <x:c r="AA2" s="27" t="s"/>
+      <x:c r="AB2" s="30" t="s"/>
+      <x:c r="AC2" s="30" t="s"/>
+      <x:c r="AD2" s="30" t="s"/>
+      <x:c r="AE2" s="30" t="s"/>
+      <x:c r="AF2" s="30" t="s"/>
+      <x:c r="AG2" s="30" t="s"/>
+      <x:c r="AH2" s="30" t="s"/>
+      <x:c r="AI2" s="30" t="s"/>
+      <x:c r="AJ2" s="30" t="s"/>
+      <x:c r="AK2" s="30" t="s"/>
+      <x:c r="AL2" s="30" t="s"/>
+      <x:c r="AM2" s="30" t="s"/>
+      <x:c r="AN2" s="34" t="s"/>
+      <x:c r="AO2" s="30" t="s"/>
+      <x:c r="AP2" s="30" t="s"/>
+      <x:c r="AQ2" s="30" t="s"/>
+      <x:c r="AR2" s="30" t="s"/>
+      <x:c r="AS2" s="30" t="s"/>
+      <x:c r="AT2" s="30" t="s"/>
+      <x:c r="AU2" s="30" t="s"/>
+      <x:c r="AV2" s="30" t="s"/>
+      <x:c r="AW2" s="30" t="s"/>
+      <x:c r="AX2" s="30" t="s"/>
+      <x:c r="AY2" s="27" t="s"/>
+      <x:c r="AZ2" s="27" t="s"/>
+      <x:c r="BA2" s="27" t="s"/>
+      <x:c r="BB2" s="27" t="s"/>
+      <x:c r="BC2" s="27" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:56" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A3" s="32" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" s="27" t="s">
+        <x:v>196</x:v>
+      </x:c>
+      <x:c r="C3" s="33" t="s"/>
+      <x:c r="D3" s="33" t="s"/>
+      <x:c r="E3" s="33" t="s"/>
+      <x:c r="F3" s="33" t="s"/>
+      <x:c r="G3" s="27" t="s"/>
+      <x:c r="H3" s="27" t="s"/>
+      <x:c r="I3" s="27" t="s"/>
+      <x:c r="J3" s="27" t="s"/>
+      <x:c r="K3" s="27" t="s"/>
+      <x:c r="L3" s="27" t="s"/>
+      <x:c r="M3" s="27" t="s"/>
+      <x:c r="N3" s="27" t="s"/>
+      <x:c r="O3" s="27" t="s"/>
+      <x:c r="P3" s="27" t="s"/>
+      <x:c r="Q3" s="27" t="s"/>
+      <x:c r="R3" s="27" t="s"/>
+      <x:c r="S3" s="27" t="s"/>
+      <x:c r="T3" s="27" t="s"/>
+      <x:c r="U3" s="27" t="s"/>
+      <x:c r="V3" s="27" t="s"/>
+      <x:c r="W3" s="27" t="s"/>
+      <x:c r="X3" s="27" t="s"/>
+      <x:c r="Y3" s="27" t="s"/>
+      <x:c r="Z3" s="27" t="s"/>
+      <x:c r="AA3" s="27" t="s"/>
+      <x:c r="AB3" s="30" t="s"/>
+      <x:c r="AC3" s="30" t="s"/>
+      <x:c r="AD3" s="30" t="s"/>
+      <x:c r="AE3" s="30" t="s"/>
+      <x:c r="AF3" s="30" t="s"/>
+      <x:c r="AG3" s="30" t="s"/>
+      <x:c r="AH3" s="30" t="s"/>
+      <x:c r="AI3" s="30" t="s"/>
+      <x:c r="AJ3" s="30" t="s"/>
+      <x:c r="AK3" s="30" t="s"/>
+      <x:c r="AL3" s="30" t="s"/>
+      <x:c r="AM3" s="30" t="s"/>
+      <x:c r="AN3" s="30" t="s"/>
+      <x:c r="AO3" s="30" t="s"/>
+      <x:c r="AP3" s="30" t="s"/>
+      <x:c r="AQ3" s="30" t="s"/>
+      <x:c r="AR3" s="30" t="s"/>
+      <x:c r="AS3" s="30" t="s"/>
+      <x:c r="AT3" s="30" t="s"/>
+      <x:c r="AU3" s="30" t="s"/>
+      <x:c r="AV3" s="30" t="s"/>
+      <x:c r="AW3" s="30" t="s"/>
+      <x:c r="AX3" s="30" t="s"/>
+      <x:c r="AY3" s="27" t="s"/>
+      <x:c r="AZ3" s="27" t="s"/>
+      <x:c r="BA3" s="27" t="s"/>
+      <x:c r="BB3" s="27" t="s"/>
+      <x:c r="BC3" s="27" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:56" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A4" s="32" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B4" s="27" t="s">
+        <x:v>319</x:v>
+      </x:c>
+      <x:c r="C4" s="33" t="s"/>
+      <x:c r="D4" s="33" t="s"/>
+      <x:c r="E4" s="33" t="s"/>
+      <x:c r="F4" s="33" t="s"/>
+      <x:c r="G4" s="27" t="s"/>
+      <x:c r="H4" s="27" t="s"/>
+      <x:c r="I4" s="27" t="s"/>
+      <x:c r="J4" s="27" t="s"/>
+      <x:c r="K4" s="27" t="s"/>
+      <x:c r="L4" s="27" t="s"/>
+      <x:c r="M4" s="27" t="s"/>
+      <x:c r="N4" s="27" t="s"/>
+      <x:c r="O4" s="27" t="s"/>
+      <x:c r="P4" s="27" t="s"/>
+      <x:c r="Q4" s="27" t="s"/>
+      <x:c r="R4" s="27" t="s"/>
+      <x:c r="S4" s="27" t="s"/>
+      <x:c r="T4" s="27" t="s"/>
+      <x:c r="U4" s="27" t="s"/>
+      <x:c r="V4" s="27" t="s"/>
+      <x:c r="W4" s="27" t="s"/>
+      <x:c r="X4" s="27" t="s"/>
+      <x:c r="Y4" s="27" t="s"/>
+      <x:c r="Z4" s="27" t="s"/>
+      <x:c r="AA4" s="27" t="s"/>
+      <x:c r="AB4" s="30" t="s"/>
+      <x:c r="AC4" s="30" t="s"/>
+      <x:c r="AD4" s="30" t="s"/>
+      <x:c r="AE4" s="30" t="s"/>
+      <x:c r="AF4" s="30" t="s"/>
+      <x:c r="AG4" s="30" t="s"/>
+      <x:c r="AH4" s="30" t="s"/>
+      <x:c r="AI4" s="30" t="s"/>
+      <x:c r="AJ4" s="30" t="s"/>
+      <x:c r="AK4" s="30" t="s"/>
+      <x:c r="AL4" s="30" t="s"/>
+      <x:c r="AM4" s="30" t="s"/>
+      <x:c r="AN4" s="30" t="s"/>
+      <x:c r="AO4" s="30" t="s"/>
+      <x:c r="AP4" s="30" t="s"/>
+      <x:c r="AQ4" s="30" t="s"/>
+      <x:c r="AR4" s="30" t="s"/>
+      <x:c r="AS4" s="30" t="s"/>
+      <x:c r="AT4" s="30" t="s"/>
+      <x:c r="AU4" s="30" t="s"/>
+      <x:c r="AV4" s="30" t="s"/>
+      <x:c r="AW4" s="30" t="s"/>
+      <x:c r="AX4" s="30" t="s"/>
+      <x:c r="AY4" s="27" t="s"/>
+      <x:c r="AZ4" s="27" t="s"/>
+      <x:c r="BA4" s="27" t="s"/>
+      <x:c r="BB4" s="27" t="s"/>
+      <x:c r="BC4" s="27" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:56" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A5" s="32" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B5" s="27" t="s"/>
+      <x:c r="C5" s="33" t="s"/>
+      <x:c r="D5" s="33" t="s"/>
+      <x:c r="E5" s="33" t="s"/>
+      <x:c r="F5" s="33" t="s"/>
+      <x:c r="G5" s="27" t="s"/>
+      <x:c r="H5" s="27" t="s"/>
+      <x:c r="I5" s="27" t="s"/>
+      <x:c r="J5" s="27" t="s"/>
+      <x:c r="K5" s="27" t="s"/>
+      <x:c r="L5" s="27" t="s"/>
+      <x:c r="M5" s="27" t="s"/>
+      <x:c r="N5" s="27" t="s"/>
+      <x:c r="O5" s="27" t="s"/>
+      <x:c r="P5" s="27" t="s"/>
+      <x:c r="Q5" s="27" t="s"/>
+      <x:c r="R5" s="27" t="s"/>
+      <x:c r="S5" s="27" t="s"/>
+      <x:c r="T5" s="27" t="s"/>
+      <x:c r="U5" s="27" t="s"/>
+      <x:c r="V5" s="27" t="s"/>
+      <x:c r="W5" s="27" t="s"/>
+      <x:c r="X5" s="27" t="s"/>
+      <x:c r="Y5" s="27" t="s"/>
+      <x:c r="Z5" s="27" t="s"/>
+      <x:c r="AA5" s="27" t="s"/>
+      <x:c r="AB5" s="30" t="s"/>
+      <x:c r="AC5" s="30" t="s"/>
+      <x:c r="AD5" s="30" t="s"/>
+      <x:c r="AE5" s="30" t="s"/>
+      <x:c r="AF5" s="30" t="s"/>
+      <x:c r="AG5" s="30" t="s"/>
+      <x:c r="AH5" s="30" t="s"/>
+      <x:c r="AI5" s="30" t="s"/>
+      <x:c r="AJ5" s="30" t="s"/>
+      <x:c r="AK5" s="30" t="s"/>
+      <x:c r="AL5" s="30" t="s"/>
+      <x:c r="AM5" s="30" t="s"/>
+      <x:c r="AN5" s="30" t="s"/>
+      <x:c r="AO5" s="30" t="s"/>
+      <x:c r="AP5" s="30" t="s"/>
+      <x:c r="AQ5" s="30" t="s"/>
+      <x:c r="AR5" s="30" t="s"/>
+      <x:c r="AS5" s="30" t="s"/>
+      <x:c r="AT5" s="30" t="s"/>
+      <x:c r="AU5" s="30" t="s"/>
+      <x:c r="AV5" s="30" t="s"/>
+      <x:c r="AW5" s="30" t="s"/>
+      <x:c r="AX5" s="30" t="s"/>
+      <x:c r="AY5" s="27" t="s"/>
+      <x:c r="AZ5" s="27" t="s"/>
+      <x:c r="BA5" s="27" t="s"/>
+      <x:c r="BB5" s="27" t="s"/>
+      <x:c r="BC5" s="27" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:56" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A6" s="32" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B6" s="27" t="s">
+        <x:v>198</x:v>
+      </x:c>
+      <x:c r="C6" s="33" t="s"/>
+      <x:c r="D6" s="33" t="s"/>
+      <x:c r="E6" s="33" t="s"/>
+      <x:c r="F6" s="33" t="s"/>
+      <x:c r="G6" s="27" t="s"/>
+      <x:c r="H6" s="27" t="s"/>
+      <x:c r="I6" s="27" t="s"/>
+      <x:c r="J6" s="27" t="s"/>
+      <x:c r="K6" s="27" t="s"/>
+      <x:c r="L6" s="27" t="s"/>
+      <x:c r="M6" s="27" t="s"/>
+      <x:c r="N6" s="27" t="s"/>
+      <x:c r="O6" s="27" t="s"/>
+      <x:c r="P6" s="27" t="s"/>
+      <x:c r="Q6" s="27" t="s"/>
+      <x:c r="R6" s="27" t="s"/>
+      <x:c r="S6" s="27" t="s"/>
+      <x:c r="T6" s="27" t="s"/>
+      <x:c r="U6" s="27" t="s"/>
+      <x:c r="V6" s="27" t="s"/>
+      <x:c r="W6" s="27" t="s"/>
+      <x:c r="X6" s="27" t="s"/>
+      <x:c r="Y6" s="27" t="s"/>
+      <x:c r="Z6" s="27" t="s"/>
+      <x:c r="AA6" s="27" t="s"/>
+      <x:c r="AB6" s="30" t="s"/>
+      <x:c r="AC6" s="30" t="s"/>
+      <x:c r="AD6" s="30" t="s"/>
+      <x:c r="AE6" s="30" t="s"/>
+      <x:c r="AF6" s="30" t="s"/>
+      <x:c r="AG6" s="30" t="s"/>
+      <x:c r="AH6" s="30" t="s"/>
+      <x:c r="AI6" s="30" t="s"/>
+      <x:c r="AJ6" s="30" t="s"/>
+      <x:c r="AK6" s="30" t="s"/>
+      <x:c r="AL6" s="30" t="s"/>
+      <x:c r="AM6" s="30" t="s"/>
+      <x:c r="AN6" s="30" t="s"/>
+      <x:c r="AO6" s="30" t="s"/>
+      <x:c r="AP6" s="30" t="s"/>
+      <x:c r="AQ6" s="30" t="s"/>
+      <x:c r="AR6" s="30" t="s"/>
+      <x:c r="AS6" s="30" t="s"/>
+      <x:c r="AT6" s="30" t="s"/>
+      <x:c r="AU6" s="30" t="s"/>
+      <x:c r="AV6" s="30" t="s"/>
+      <x:c r="AW6" s="30" t="s"/>
+      <x:c r="AX6" s="30" t="s"/>
+      <x:c r="AY6" s="27" t="s"/>
+      <x:c r="AZ6" s="27" t="s"/>
+      <x:c r="BA6" s="27" t="s"/>
+      <x:c r="BB6" s="27" t="s"/>
+      <x:c r="BC6" s="27" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:56" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A7" s="32" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B7" s="35" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C7" s="33" t="s"/>
+      <x:c r="D7" s="33" t="s"/>
+      <x:c r="E7" s="33" t="s"/>
+      <x:c r="F7" s="33" t="s"/>
+      <x:c r="G7" s="27" t="s"/>
+      <x:c r="H7" s="27" t="s"/>
+      <x:c r="I7" s="27" t="s"/>
+      <x:c r="J7" s="27" t="s"/>
+      <x:c r="K7" s="27" t="s"/>
+      <x:c r="L7" s="27" t="s"/>
+      <x:c r="M7" s="27" t="s"/>
+      <x:c r="N7" s="27" t="s"/>
+      <x:c r="O7" s="27" t="s"/>
+      <x:c r="P7" s="27" t="s"/>
+      <x:c r="Q7" s="27" t="s"/>
+      <x:c r="R7" s="27" t="s"/>
+      <x:c r="S7" s="27" t="s"/>
+      <x:c r="T7" s="27" t="s"/>
+      <x:c r="U7" s="27" t="s"/>
+      <x:c r="V7" s="27" t="s"/>
+      <x:c r="W7" s="27" t="s"/>
+      <x:c r="X7" s="27" t="s"/>
+      <x:c r="Y7" s="27" t="s"/>
+      <x:c r="Z7" s="27" t="s"/>
+      <x:c r="AA7" s="27" t="s"/>
+      <x:c r="AB7" s="36" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="AC7" s="30" t="s"/>
+      <x:c r="AD7" s="30" t="s"/>
+      <x:c r="AE7" s="30" t="s"/>
+      <x:c r="AF7" s="30" t="s"/>
+      <x:c r="AG7" s="30" t="s"/>
+      <x:c r="AH7" s="30" t="s"/>
+      <x:c r="AI7" s="30" t="s"/>
+      <x:c r="AJ7" s="30" t="s"/>
+      <x:c r="AK7" s="30" t="s"/>
+      <x:c r="AL7" s="30" t="s"/>
+      <x:c r="AM7" s="30" t="s"/>
+      <x:c r="AN7" s="30" t="s"/>
+      <x:c r="AO7" s="30" t="s"/>
+      <x:c r="AP7" s="30" t="s"/>
+      <x:c r="AQ7" s="30" t="s"/>
+      <x:c r="AR7" s="30" t="s"/>
+      <x:c r="AS7" s="30" t="s"/>
+      <x:c r="AT7" s="30" t="s"/>
+      <x:c r="AU7" s="30" t="s"/>
+      <x:c r="AV7" s="30" t="s"/>
+      <x:c r="AW7" s="30" t="s"/>
+      <x:c r="AX7" s="30" t="s"/>
+      <x:c r="AY7" s="27" t="s"/>
+      <x:c r="AZ7" s="27" t="s"/>
+      <x:c r="BA7" s="27" t="s"/>
+      <x:c r="BB7" s="27" t="s"/>
+      <x:c r="BC7" s="27" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:56" customFormat="1" ht="13.5" customHeight="1">
+      <x:c r="A8" s="37" t="s"/>
+      <x:c r="B8" s="37" t="s"/>
+      <x:c r="C8" s="37" t="s"/>
+      <x:c r="D8" s="37" t="s"/>
+      <x:c r="E8" s="37" t="s"/>
+      <x:c r="F8" s="37" t="s"/>
+      <x:c r="G8" s="37" t="s"/>
+      <x:c r="H8" s="37" t="s"/>
+      <x:c r="I8" s="37" t="s"/>
+      <x:c r="J8" s="37" t="s"/>
+      <x:c r="K8" s="37" t="s"/>
+      <x:c r="L8" s="37" t="s"/>
+      <x:c r="M8" s="37" t="s"/>
+      <x:c r="N8" s="37" t="s"/>
+      <x:c r="O8" s="37" t="s"/>
+      <x:c r="P8" s="37" t="s"/>
+      <x:c r="Q8" s="37" t="s"/>
+      <x:c r="R8" s="37" t="s"/>
+      <x:c r="S8" s="37" t="s"/>
+      <x:c r="T8" s="37" t="s"/>
+      <x:c r="U8" s="37" t="s"/>
+      <x:c r="V8" s="37" t="s"/>
+      <x:c r="W8" s="37" t="s"/>
+      <x:c r="X8" s="37" t="s"/>
+      <x:c r="Y8" s="37" t="s"/>
+      <x:c r="Z8" s="37" t="s"/>
+      <x:c r="AA8" s="37" t="s"/>
+      <x:c r="AB8" s="38" t="s"/>
+      <x:c r="AC8" s="38" t="s"/>
+      <x:c r="AD8" s="38" t="s"/>
+      <x:c r="AE8" s="38" t="s"/>
+      <x:c r="AF8" s="38" t="s"/>
+      <x:c r="AG8" s="38" t="s"/>
+      <x:c r="AH8" s="38" t="s"/>
+      <x:c r="AI8" s="38" t="s"/>
+      <x:c r="AJ8" s="38" t="s"/>
+      <x:c r="AK8" s="38" t="s"/>
+      <x:c r="AL8" s="38" t="s"/>
+      <x:c r="AM8" s="38" t="s"/>
+      <x:c r="AN8" s="38" t="s"/>
+      <x:c r="AO8" s="38" t="s"/>
+      <x:c r="AP8" s="38" t="s"/>
+      <x:c r="AQ8" s="38" t="s"/>
+      <x:c r="AR8" s="38" t="s"/>
+      <x:c r="AS8" s="38" t="s"/>
+      <x:c r="AT8" s="38" t="s"/>
+      <x:c r="AU8" s="38" t="s"/>
+      <x:c r="AV8" s="38" t="s"/>
+      <x:c r="AW8" s="38" t="s"/>
+      <x:c r="AX8" s="38" t="s"/>
+      <x:c r="AY8" s="37" t="s"/>
+      <x:c r="AZ8" s="37" t="s"/>
+      <x:c r="BA8" s="37" t="s"/>
+      <x:c r="BB8" s="37" t="s"/>
+      <x:c r="BC8" s="37" t="s"/>
+      <x:c r="BD8" s="37" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:56" customFormat="1" ht="51.75" customHeight="1">
+      <x:c r="A9" s="39" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B9" s="39" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C9" s="39" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D9" s="39" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E9" s="39" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F9" s="39" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G9" s="39" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H9" s="40" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="I9" s="40" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J9" s="41" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="K9" s="41" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="L9" s="41" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="M9" s="41" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="N9" s="41" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="O9" s="42" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="P9" s="43" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="Q9" s="41" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="R9" s="44" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="S9" s="40" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="T9" s="41" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="U9" s="40" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="V9" s="39" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="W9" s="40" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="X9" s="40" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="Y9" s="40" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="Z9" s="40" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="AA9" s="41" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="AB9" s="45" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="AC9" s="41" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="AD9" s="45" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="AE9" s="41" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="AF9" s="45" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="AG9" s="45" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="AH9" s="45" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="AI9" s="41" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AJ9" s="41" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AK9" s="45" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="AL9" s="45" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AM9" s="45" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AN9" s="46" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AO9" s="41" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="AP9" s="44" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="AQ9" s="47" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="AR9" s="43" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="AS9" s="41" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="AT9" s="41" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="AU9" s="41" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="AV9" s="41" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="AW9" s="41" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="AX9" s="41" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="AY9" s="44" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="AZ9" s="47" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="BA9" s="48" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="BB9" s="49" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="BC9" s="50" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="BD9" s="51" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:56">
+      <x:c r="A10" s="27" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="B10" s="27" t="s"/>
+      <x:c r="C10" s="27" t="s"/>
+      <x:c r="D10" s="27" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="E10" s="27" t="s"/>
+      <x:c r="F10" s="27" t="s"/>
+      <x:c r="G10" s="27" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="H10" s="27" t="s"/>
+      <x:c r="I10" s="27" t="s"/>
+      <x:c r="J10" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K10" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L10" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M10" s="27" t="s">
+        <x:v>322</x:v>
+      </x:c>
+      <x:c r="N10" s="27" t="s">
+        <x:v>323</x:v>
+      </x:c>
+      <x:c r="O10" s="27" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="V10" s="27" t="s">
+        <x:v>325</x:v>
+      </x:c>
+      <x:c r="W10" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X10" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y10" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z10" s="52" t="n">
+        <x:v>875</x:v>
+      </x:c>
+      <x:c r="AA10" s="52" t="n">
+        <x:v>525</x:v>
+      </x:c>
+      <x:c r="AB10" s="52">
+        <x:f>AA10</x:f>
+      </x:c>
+      <x:c r="AC10" s="52" t="s"/>
+      <x:c r="AD10" s="52">
+        <x:f>AC10</x:f>
+      </x:c>
+      <x:c r="AE10" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF10" s="52">
+        <x:f>AE10</x:f>
+      </x:c>
+      <x:c r="AG10" s="52">
+        <x:f>+AA10-AC10+AE10</x:f>
+      </x:c>
+      <x:c r="AH10" s="52">
+        <x:f>+AB10-AD10+AF10</x:f>
+      </x:c>
+      <x:c r="AI10" s="52" t="s"/>
+      <x:c r="AJ10" s="52" t="s"/>
+      <x:c r="AK10" s="52">
+        <x:f>+AI10+AJ10</x:f>
+      </x:c>
+      <x:c r="AL10" s="52">
+        <x:f>+AB10-AD10+AI10</x:f>
+      </x:c>
+      <x:c r="AM10" s="52">
+        <x:f>+AF10+AJ10</x:f>
+      </x:c>
+      <x:c r="AN10" s="52">
+        <x:f>+AL10+AM10</x:f>
+      </x:c>
+      <x:c r="AO10" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP10" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV10" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW10" s="27" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:56">
+      <x:c r="A11" s="27" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="B11" s="27" t="s"/>
+      <x:c r="C11" s="27" t="s"/>
+      <x:c r="D11" s="27" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="E11" s="27" t="s"/>
+      <x:c r="F11" s="27" t="s"/>
+      <x:c r="G11" s="27" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="H11" s="27" t="s"/>
+      <x:c r="I11" s="27" t="s"/>
+      <x:c r="J11" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K11" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L11" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M11" s="27" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="N11" s="27" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="O11" s="27" t="s">
+        <x:v>328</x:v>
+      </x:c>
+      <x:c r="V11" s="27" t="s">
+        <x:v>329</x:v>
+      </x:c>
+      <x:c r="W11" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X11" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y11" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z11" s="52" t="n">
+        <x:v>362.8</x:v>
+      </x:c>
+      <x:c r="AA11" s="52" t="n">
+        <x:v>259.176</x:v>
+      </x:c>
+      <x:c r="AB11" s="52">
+        <x:f>AA11</x:f>
+      </x:c>
+      <x:c r="AC11" s="52" t="s"/>
+      <x:c r="AD11" s="52">
+        <x:f>AC11</x:f>
+      </x:c>
+      <x:c r="AE11" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF11" s="52">
+        <x:f>AE11</x:f>
+      </x:c>
+      <x:c r="AG11" s="52">
+        <x:f>+AA11-AC11+AE11</x:f>
+      </x:c>
+      <x:c r="AH11" s="52">
+        <x:f>+AB11-AD11+AF11</x:f>
+      </x:c>
+      <x:c r="AI11" s="52" t="s"/>
+      <x:c r="AJ11" s="52" t="s"/>
+      <x:c r="AK11" s="52">
+        <x:f>+AI11+AJ11</x:f>
+      </x:c>
+      <x:c r="AL11" s="52">
+        <x:f>+AB11-AD11+AI11</x:f>
+      </x:c>
+      <x:c r="AM11" s="52">
+        <x:f>+AF11+AJ11</x:f>
+      </x:c>
+      <x:c r="AN11" s="52">
+        <x:f>+AL11+AM11</x:f>
+      </x:c>
+      <x:c r="AO11" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP11" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV11" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW11" s="27" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:56">
+      <x:c r="A12" s="27" t="s">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="B12" s="27" t="s"/>
+      <x:c r="C12" s="27" t="s"/>
+      <x:c r="D12" s="27" t="s">
+        <x:v>331</x:v>
+      </x:c>
+      <x:c r="E12" s="27" t="s"/>
+      <x:c r="F12" s="27" t="s"/>
+      <x:c r="G12" s="27" t="s">
+        <x:v>332</x:v>
+      </x:c>
+      <x:c r="H12" s="27" t="s"/>
+      <x:c r="I12" s="27" t="s"/>
+      <x:c r="J12" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K12" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L12" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M12" s="27" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="N12" s="27" t="s">
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="O12" s="27" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="V12" s="27" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="W12" s="27" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="X12" s="27" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="Y12" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z12" s="52" t="n">
+        <x:v>19983.3333</x:v>
+      </x:c>
+      <x:c r="AA12" s="52" t="n">
+        <x:v>9991.6633</x:v>
+      </x:c>
+      <x:c r="AB12" s="52">
+        <x:f>AA12</x:f>
+      </x:c>
+      <x:c r="AC12" s="52" t="s"/>
+      <x:c r="AD12" s="52">
+        <x:f>AC12</x:f>
+      </x:c>
+      <x:c r="AE12" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF12" s="52">
+        <x:f>AE12</x:f>
+      </x:c>
+      <x:c r="AG12" s="52">
+        <x:f>+AA12-AC12+AE12</x:f>
+      </x:c>
+      <x:c r="AH12" s="52">
+        <x:f>+AB12-AD12+AF12</x:f>
+      </x:c>
+      <x:c r="AI12" s="52" t="s"/>
+      <x:c r="AJ12" s="52" t="s"/>
+      <x:c r="AK12" s="52">
+        <x:f>+AI12+AJ12</x:f>
+      </x:c>
+      <x:c r="AL12" s="52">
+        <x:f>+AB12-AD12+AI12</x:f>
+      </x:c>
+      <x:c r="AM12" s="52">
+        <x:f>+AF12+AJ12</x:f>
+      </x:c>
+      <x:c r="AN12" s="52">
+        <x:f>+AL12+AM12</x:f>
+      </x:c>
+      <x:c r="AO12" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP12" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV12" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW12" s="27" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:56">
+      <x:c r="A13" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B13" s="27" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="C13" s="27" t="s"/>
+      <x:c r="D13" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E13" s="27" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="F13" s="27" t="s"/>
+      <x:c r="G13" s="27" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="H13" s="27" t="s"/>
+      <x:c r="I13" s="27" t="s"/>
+      <x:c r="J13" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K13" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L13" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M13" s="27" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="N13" s="27" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="O13" s="27" t="s">
+        <x:v>339</x:v>
+      </x:c>
+      <x:c r="V13" s="27" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="W13" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X13" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y13" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z13" s="52" t="n">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="AA13" s="52" t="n">
+        <x:v>47.52</x:v>
+      </x:c>
+      <x:c r="AB13" s="52">
+        <x:f>AA13</x:f>
+      </x:c>
+      <x:c r="AC13" s="52" t="s"/>
+      <x:c r="AD13" s="52">
+        <x:f>AC13</x:f>
+      </x:c>
+      <x:c r="AE13" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF13" s="52">
+        <x:f>AE13</x:f>
+      </x:c>
+      <x:c r="AG13" s="52">
+        <x:f>+AA13-AC13+AE13</x:f>
+      </x:c>
+      <x:c r="AH13" s="52">
+        <x:f>+AB13-AD13+AF13</x:f>
+      </x:c>
+      <x:c r="AI13" s="52" t="s"/>
+      <x:c r="AJ13" s="52" t="s"/>
+      <x:c r="AK13" s="52">
+        <x:f>+AI13+AJ13</x:f>
+      </x:c>
+      <x:c r="AL13" s="52">
+        <x:f>+AB13-AD13+AI13</x:f>
+      </x:c>
+      <x:c r="AM13" s="52">
+        <x:f>+AF13+AJ13</x:f>
+      </x:c>
+      <x:c r="AN13" s="52">
+        <x:f>+AL13+AM13</x:f>
+      </x:c>
+      <x:c r="AO13" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP13" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV13" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW13" s="27" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:56">
+      <x:c r="A14" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B14" s="27" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="C14" s="27" t="s"/>
+      <x:c r="D14" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E14" s="27" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="F14" s="27" t="s"/>
+      <x:c r="G14" s="27" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="H14" s="27" t="s"/>
+      <x:c r="I14" s="27" t="s"/>
+      <x:c r="J14" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K14" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L14" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M14" s="27" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="N14" s="27" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="O14" s="27" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="V14" s="27" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="W14" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X14" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y14" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z14" s="52" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="AA14" s="52" t="n">
+        <x:v>480</x:v>
+      </x:c>
+      <x:c r="AB14" s="52">
+        <x:f>AA14</x:f>
+      </x:c>
+      <x:c r="AC14" s="52" t="s"/>
+      <x:c r="AD14" s="52">
+        <x:f>AC14</x:f>
+      </x:c>
+      <x:c r="AE14" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF14" s="52">
+        <x:f>AE14</x:f>
+      </x:c>
+      <x:c r="AG14" s="52">
+        <x:f>+AA14-AC14+AE14</x:f>
+      </x:c>
+      <x:c r="AH14" s="52">
+        <x:f>+AB14-AD14+AF14</x:f>
+      </x:c>
+      <x:c r="AI14" s="52" t="s"/>
+      <x:c r="AJ14" s="52" t="s"/>
+      <x:c r="AK14" s="52">
+        <x:f>+AI14+AJ14</x:f>
+      </x:c>
+      <x:c r="AL14" s="52">
+        <x:f>+AB14-AD14+AI14</x:f>
+      </x:c>
+      <x:c r="AM14" s="52">
+        <x:f>+AF14+AJ14</x:f>
+      </x:c>
+      <x:c r="AN14" s="52">
+        <x:f>+AL14+AM14</x:f>
+      </x:c>
+      <x:c r="AO14" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP14" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV14" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW14" s="27" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:56">
+      <x:c r="A15" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B15" s="27" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="C15" s="27" t="s"/>
+      <x:c r="D15" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E15" s="27" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="F15" s="27" t="s"/>
+      <x:c r="G15" s="27" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="H15" s="27" t="s"/>
+      <x:c r="I15" s="27" t="s"/>
+      <x:c r="J15" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K15" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L15" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M15" s="27" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="N15" s="27" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="O15" s="27" t="s">
+        <x:v>343</x:v>
+      </x:c>
+      <x:c r="V15" s="27" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="W15" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X15" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y15" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z15" s="52" t="n">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="AA15" s="52" t="n">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="AB15" s="52">
+        <x:f>AA15</x:f>
+      </x:c>
+      <x:c r="AC15" s="52" t="s"/>
+      <x:c r="AD15" s="52">
+        <x:f>AC15</x:f>
+      </x:c>
+      <x:c r="AE15" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF15" s="52">
+        <x:f>AE15</x:f>
+      </x:c>
+      <x:c r="AG15" s="52">
+        <x:f>+AA15-AC15+AE15</x:f>
+      </x:c>
+      <x:c r="AH15" s="52">
+        <x:f>+AB15-AD15+AF15</x:f>
+      </x:c>
+      <x:c r="AI15" s="52" t="s"/>
+      <x:c r="AJ15" s="52" t="s"/>
+      <x:c r="AK15" s="52">
+        <x:f>+AI15+AJ15</x:f>
+      </x:c>
+      <x:c r="AL15" s="52">
+        <x:f>+AB15-AD15+AI15</x:f>
+      </x:c>
+      <x:c r="AM15" s="52">
+        <x:f>+AF15+AJ15</x:f>
+      </x:c>
+      <x:c r="AN15" s="52">
+        <x:f>+AL15+AM15</x:f>
+      </x:c>
+      <x:c r="AO15" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP15" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV15" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW15" s="27" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:56">
+      <x:c r="A16" s="27" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="B16" s="27" t="s"/>
+      <x:c r="C16" s="27" t="s"/>
+      <x:c r="D16" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E16" s="27" t="s"/>
+      <x:c r="F16" s="27" t="s"/>
+      <x:c r="G16" s="27" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="H16" s="27" t="s"/>
+      <x:c r="I16" s="27" t="s"/>
+      <x:c r="J16" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K16" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L16" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M16" s="27" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="N16" s="27" t="s">
+        <x:v>346</x:v>
+      </x:c>
+      <x:c r="O16" s="27" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="V16" s="27" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="W16" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X16" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y16" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z16" s="52" t="n">
+        <x:v>500</x:v>
+      </x:c>
+      <x:c r="AA16" s="52" t="n">
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="AB16" s="52">
+        <x:f>AA16</x:f>
+      </x:c>
+      <x:c r="AC16" s="52" t="s"/>
+      <x:c r="AD16" s="52">
+        <x:f>AC16</x:f>
+      </x:c>
+      <x:c r="AE16" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF16" s="52">
+        <x:f>AE16</x:f>
+      </x:c>
+      <x:c r="AG16" s="52">
+        <x:f>+AA16-AC16+AE16</x:f>
+      </x:c>
+      <x:c r="AH16" s="52">
+        <x:f>+AB16-AD16+AF16</x:f>
+      </x:c>
+      <x:c r="AI16" s="52" t="s"/>
+      <x:c r="AJ16" s="52" t="s"/>
+      <x:c r="AK16" s="52">
+        <x:f>+AI16+AJ16</x:f>
+      </x:c>
+      <x:c r="AL16" s="52">
+        <x:f>+AB16-AD16+AI16</x:f>
+      </x:c>
+      <x:c r="AM16" s="52">
+        <x:f>+AF16+AJ16</x:f>
+      </x:c>
+      <x:c r="AN16" s="52">
+        <x:f>+AL16+AM16</x:f>
+      </x:c>
+      <x:c r="AO16" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP16" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV16" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW16" s="27" t="s"/>
+    </x:row>
+    <x:row r="17" spans="1:56">
+      <x:c r="A17" s="27" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="B17" s="27" t="s"/>
+      <x:c r="C17" s="27" t="s"/>
+      <x:c r="D17" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E17" s="27" t="s"/>
+      <x:c r="F17" s="27" t="s"/>
+      <x:c r="G17" s="27" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="H17" s="27" t="s"/>
+      <x:c r="I17" s="27" t="s"/>
+      <x:c r="J17" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K17" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L17" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M17" s="27" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="N17" s="27" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="O17" s="27" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="V17" s="27" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="W17" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X17" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y17" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z17" s="52" t="n">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="AA17" s="52" t="n">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="AB17" s="52">
+        <x:f>AA17</x:f>
+      </x:c>
+      <x:c r="AC17" s="52" t="s"/>
+      <x:c r="AD17" s="52">
+        <x:f>AC17</x:f>
+      </x:c>
+      <x:c r="AE17" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF17" s="52">
+        <x:f>AE17</x:f>
+      </x:c>
+      <x:c r="AG17" s="52">
+        <x:f>+AA17-AC17+AE17</x:f>
+      </x:c>
+      <x:c r="AH17" s="52">
+        <x:f>+AB17-AD17+AF17</x:f>
+      </x:c>
+      <x:c r="AI17" s="52" t="s"/>
+      <x:c r="AJ17" s="52" t="s"/>
+      <x:c r="AK17" s="52">
+        <x:f>+AI17+AJ17</x:f>
+      </x:c>
+      <x:c r="AL17" s="52">
+        <x:f>+AB17-AD17+AI17</x:f>
+      </x:c>
+      <x:c r="AM17" s="52">
+        <x:f>+AF17+AJ17</x:f>
+      </x:c>
+      <x:c r="AN17" s="52">
+        <x:f>+AL17+AM17</x:f>
+      </x:c>
+      <x:c r="AO17" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP17" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV17" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW17" s="27" t="s"/>
+    </x:row>
+    <x:row r="18" spans="1:56">
+      <x:c r="A18" s="27" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="B18" s="27" t="s"/>
+      <x:c r="C18" s="27" t="s"/>
+      <x:c r="D18" s="27" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="E18" s="27" t="s"/>
+      <x:c r="F18" s="27" t="s"/>
+      <x:c r="G18" s="27" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="H18" s="27" t="s"/>
+      <x:c r="I18" s="27" t="s"/>
+      <x:c r="J18" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K18" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L18" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M18" s="27" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="N18" s="27" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="O18" s="27" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="V18" s="27" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="W18" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X18" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y18" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z18" s="52" t="n">
+        <x:v>743</x:v>
+      </x:c>
+      <x:c r="AA18" s="52" t="n">
+        <x:v>356.64</x:v>
+      </x:c>
+      <x:c r="AB18" s="52">
+        <x:f>AA18</x:f>
+      </x:c>
+      <x:c r="AC18" s="52" t="s"/>
+      <x:c r="AD18" s="52">
+        <x:f>AC18</x:f>
+      </x:c>
+      <x:c r="AE18" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF18" s="52">
+        <x:f>AE18</x:f>
+      </x:c>
+      <x:c r="AG18" s="52">
+        <x:f>+AA18-AC18+AE18</x:f>
+      </x:c>
+      <x:c r="AH18" s="52">
+        <x:f>+AB18-AD18+AF18</x:f>
+      </x:c>
+      <x:c r="AI18" s="52" t="s"/>
+      <x:c r="AJ18" s="52" t="s"/>
+      <x:c r="AK18" s="52">
+        <x:f>+AI18+AJ18</x:f>
+      </x:c>
+      <x:c r="AL18" s="52">
+        <x:f>+AB18-AD18+AI18</x:f>
+      </x:c>
+      <x:c r="AM18" s="52">
+        <x:f>+AF18+AJ18</x:f>
+      </x:c>
+      <x:c r="AN18" s="52">
+        <x:f>+AL18+AM18</x:f>
+      </x:c>
+      <x:c r="AO18" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP18" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV18" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW18" s="27" t="s"/>
+    </x:row>
+    <x:row r="19" spans="1:56">
+      <x:c r="A19" s="27" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="B19" s="27" t="s"/>
+      <x:c r="C19" s="27" t="s"/>
+      <x:c r="D19" s="27" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="E19" s="27" t="s"/>
+      <x:c r="F19" s="27" t="s"/>
+      <x:c r="G19" s="27" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="H19" s="27" t="s"/>
+      <x:c r="I19" s="27" t="s"/>
+      <x:c r="J19" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K19" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L19" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M19" s="27" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="N19" s="27" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="O19" s="27" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="V19" s="27" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="W19" s="27" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="X19" s="27" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="Y19" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z19" s="52" t="n">
+        <x:v>83.3333</x:v>
+      </x:c>
+      <x:c r="AA19" s="52" t="n">
+        <x:v>83.3333</x:v>
+      </x:c>
+      <x:c r="AB19" s="52">
+        <x:f>AA19</x:f>
+      </x:c>
+      <x:c r="AC19" s="52" t="s"/>
+      <x:c r="AD19" s="52">
+        <x:f>AC19</x:f>
+      </x:c>
+      <x:c r="AE19" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF19" s="52">
+        <x:f>AE19</x:f>
+      </x:c>
+      <x:c r="AG19" s="52">
+        <x:f>+AA19-AC19+AE19</x:f>
+      </x:c>
+      <x:c r="AH19" s="52">
+        <x:f>+AB19-AD19+AF19</x:f>
+      </x:c>
+      <x:c r="AI19" s="52" t="s"/>
+      <x:c r="AJ19" s="52" t="s"/>
+      <x:c r="AK19" s="52">
+        <x:f>+AI19+AJ19</x:f>
+      </x:c>
+      <x:c r="AL19" s="52">
+        <x:f>+AB19-AD19+AI19</x:f>
+      </x:c>
+      <x:c r="AM19" s="52">
+        <x:f>+AF19+AJ19</x:f>
+      </x:c>
+      <x:c r="AN19" s="52">
+        <x:f>+AL19+AM19</x:f>
+      </x:c>
+      <x:c r="AO19" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP19" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV19" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW19" s="27" t="s"/>
+    </x:row>
+    <x:row r="20" spans="1:56">
+      <x:c r="A20" s="27" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="B20" s="27" t="s"/>
+      <x:c r="C20" s="27" t="s"/>
+      <x:c r="D20" s="27" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="E20" s="27" t="s"/>
+      <x:c r="F20" s="27" t="s"/>
+      <x:c r="G20" s="27" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="H20" s="27" t="s"/>
+      <x:c r="I20" s="27" t="s"/>
+      <x:c r="J20" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K20" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L20" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M20" s="27" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="N20" s="27" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="O20" s="27" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="V20" s="27" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="W20" s="27" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="X20" s="27" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="Y20" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z20" s="52" t="n">
+        <x:v>83.3333</x:v>
+      </x:c>
+      <x:c r="AA20" s="52" t="n">
+        <x:v>83.3333</x:v>
+      </x:c>
+      <x:c r="AB20" s="52">
+        <x:f>AA20</x:f>
+      </x:c>
+      <x:c r="AC20" s="52" t="s"/>
+      <x:c r="AD20" s="52">
+        <x:f>AC20</x:f>
+      </x:c>
+      <x:c r="AE20" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF20" s="52">
+        <x:f>AE20</x:f>
+      </x:c>
+      <x:c r="AG20" s="52">
+        <x:f>+AA20-AC20+AE20</x:f>
+      </x:c>
+      <x:c r="AH20" s="52">
+        <x:f>+AB20-AD20+AF20</x:f>
+      </x:c>
+      <x:c r="AI20" s="52" t="s"/>
+      <x:c r="AJ20" s="52" t="s"/>
+      <x:c r="AK20" s="52">
+        <x:f>+AI20+AJ20</x:f>
+      </x:c>
+      <x:c r="AL20" s="52">
+        <x:f>+AB20-AD20+AI20</x:f>
+      </x:c>
+      <x:c r="AM20" s="52">
+        <x:f>+AF20+AJ20</x:f>
+      </x:c>
+      <x:c r="AN20" s="52">
+        <x:f>+AL20+AM20</x:f>
+      </x:c>
+      <x:c r="AO20" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP20" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV20" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW20" s="27" t="s"/>
+    </x:row>
+    <x:row r="21" spans="1:56">
+      <x:c r="A21" s="27" t="s">
+        <x:v>359</x:v>
+      </x:c>
+      <x:c r="B21" s="27" t="s"/>
+      <x:c r="C21" s="27" t="s"/>
+      <x:c r="D21" s="27" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="E21" s="27" t="s"/>
+      <x:c r="F21" s="27" t="s"/>
+      <x:c r="G21" s="27" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="H21" s="27" t="s"/>
+      <x:c r="I21" s="27" t="s"/>
+      <x:c r="J21" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K21" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L21" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M21" s="27" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="N21" s="27" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="O21" s="27" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="V21" s="27" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="W21" s="27" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="X21" s="27" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="Y21" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z21" s="52" t="n">
+        <x:v>83.3333</x:v>
+      </x:c>
+      <x:c r="AA21" s="52" t="n">
+        <x:v>83.3333</x:v>
+      </x:c>
+      <x:c r="AB21" s="52">
+        <x:f>AA21</x:f>
+      </x:c>
+      <x:c r="AC21" s="52" t="s"/>
+      <x:c r="AD21" s="52">
+        <x:f>AC21</x:f>
+      </x:c>
+      <x:c r="AE21" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF21" s="52">
+        <x:f>AE21</x:f>
+      </x:c>
+      <x:c r="AG21" s="52">
+        <x:f>+AA21-AC21+AE21</x:f>
+      </x:c>
+      <x:c r="AH21" s="52">
+        <x:f>+AB21-AD21+AF21</x:f>
+      </x:c>
+      <x:c r="AI21" s="52" t="s"/>
+      <x:c r="AJ21" s="52" t="s"/>
+      <x:c r="AK21" s="52">
+        <x:f>+AI21+AJ21</x:f>
+      </x:c>
+      <x:c r="AL21" s="52">
+        <x:f>+AB21-AD21+AI21</x:f>
+      </x:c>
+      <x:c r="AM21" s="52">
+        <x:f>+AF21+AJ21</x:f>
+      </x:c>
+      <x:c r="AN21" s="52">
+        <x:f>+AL21+AM21</x:f>
+      </x:c>
+      <x:c r="AO21" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP21" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV21" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW21" s="27" t="s"/>
+    </x:row>
+    <x:row r="22" spans="1:56">
+      <x:c r="A22" s="27" t="s">
+        <x:v>362</x:v>
+      </x:c>
+      <x:c r="B22" s="27" t="s"/>
+      <x:c r="C22" s="27" t="s"/>
+      <x:c r="D22" s="27" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="E22" s="27" t="s"/>
+      <x:c r="F22" s="27" t="s"/>
+      <x:c r="G22" s="27" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="H22" s="27" t="s"/>
+      <x:c r="I22" s="27" t="s"/>
+      <x:c r="J22" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K22" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L22" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M22" s="27" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="N22" s="27" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="O22" s="27" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="V22" s="27" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="W22" s="27" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="X22" s="27" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="Y22" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z22" s="52" t="n">
+        <x:v>283.3333</x:v>
+      </x:c>
+      <x:c r="AA22" s="52" t="n">
+        <x:v>283.3334</x:v>
+      </x:c>
+      <x:c r="AB22" s="52">
+        <x:f>AA22</x:f>
+      </x:c>
+      <x:c r="AC22" s="52" t="s"/>
+      <x:c r="AD22" s="52">
+        <x:f>AC22</x:f>
+      </x:c>
+      <x:c r="AE22" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF22" s="52">
+        <x:f>AE22</x:f>
+      </x:c>
+      <x:c r="AG22" s="52">
+        <x:f>+AA22-AC22+AE22</x:f>
+      </x:c>
+      <x:c r="AH22" s="52">
+        <x:f>+AB22-AD22+AF22</x:f>
+      </x:c>
+      <x:c r="AI22" s="52" t="s"/>
+      <x:c r="AJ22" s="52" t="s"/>
+      <x:c r="AK22" s="52">
+        <x:f>+AI22+AJ22</x:f>
+      </x:c>
+      <x:c r="AL22" s="52">
+        <x:f>+AB22-AD22+AI22</x:f>
+      </x:c>
+      <x:c r="AM22" s="52">
+        <x:f>+AF22+AJ22</x:f>
+      </x:c>
+      <x:c r="AN22" s="52">
+        <x:f>+AL22+AM22</x:f>
+      </x:c>
+      <x:c r="AO22" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AP22" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AV22" s="27" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="AW22" s="27" t="s"/>
+    </x:row>
+    <x:row r="23" spans="1:56">
+      <x:c r="A23" s="27" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="B23" s="27" t="s"/>
+      <x:c r="C23" s="27" t="s"/>
+      <x:c r="D23" s="27" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="E23" s="27" t="s"/>
+      <x:c r="F23" s="27" t="s"/>
+      <x:c r="G23" s="27" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="H23" s="27" t="s"/>
+      <x:c r="I23" s="27" t="s"/>
+      <x:c r="J23" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K23" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L23" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M23" s="27" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="N23" s="27" t="s">
+        <x:v>366</x:v>
+      </x:c>
+      <x:c r="O23" s="27" t="s">
+        <x:v>367</x:v>
+      </x:c>
+      <x:c r="V23" s="27" t="s">
+        <x:v>368</x:v>
+      </x:c>
+      <x:c r="W23" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X23" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y23" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z23" s="52" t="n">
+        <x:v>2062</x:v>
+      </x:c>
+      <x:c r="AA23" s="52" t="n">
+        <x:v>989.76</x:v>
+      </x:c>
+      <x:c r="AB23" s="52">
+        <x:f>AA23</x:f>
+      </x:c>
+      <x:c r="AC23" s="52" t="s"/>
+      <x:c r="AD23" s="52">
+        <x:f>AC23</x:f>
+      </x:c>
+      <x:c r="AE23" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF23" s="52">
+        <x:f>AE23</x:f>
+      </x:c>
+      <x:c r="AG23" s="52">
+        <x:f>+AA23-AC23+AE23</x:f>
+      </x:c>
+      <x:c r="AH23" s="52">
+        <x:f>+AB23-AD23+AF23</x:f>
+      </x:c>
+      <x:c r="AI23" s="52" t="s"/>
+      <x:c r="AJ23" s="52" t="s"/>
+      <x:c r="AK23" s="52">
+        <x:f>+AI23+AJ23</x:f>
+      </x:c>
+      <x:c r="AL23" s="52">
+        <x:f>+AB23-AD23+AI23</x:f>
+      </x:c>
+      <x:c r="AM23" s="52">
+        <x:f>+AF23+AJ23</x:f>
+      </x:c>
+      <x:c r="AN23" s="52">
+        <x:f>+AL23+AM23</x:f>
+      </x:c>
+      <x:c r="AO23" s="27" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="AP23" s="27" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="AV23" s="27" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="AW23" s="27" t="s"/>
+    </x:row>
+    <x:row r="24" spans="1:56">
+      <x:c r="A24" s="27" t="s">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="B24" s="27" t="s"/>
+      <x:c r="C24" s="27" t="s"/>
+      <x:c r="D24" s="27" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="E24" s="27" t="s"/>
+      <x:c r="F24" s="27" t="s"/>
+      <x:c r="G24" s="27" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="H24" s="27" t="s"/>
+      <x:c r="I24" s="27" t="s"/>
+      <x:c r="J24" s="27" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K24" s="27" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="L24" s="27" t="n">
+        <x:v>2017</x:v>
+      </x:c>
+      <x:c r="M24" s="27" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="N24" s="27" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="O24" s="27" t="s">
+        <x:v>373</x:v>
+      </x:c>
+      <x:c r="V24" s="27" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="W24" s="27" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="X24" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Y24" s="27" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="Z24" s="52" t="n">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="AA24" s="52" t="n">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="AB24" s="52">
+        <x:f>AA24</x:f>
+      </x:c>
+      <x:c r="AC24" s="52" t="s"/>
+      <x:c r="AD24" s="52">
+        <x:f>AC24</x:f>
+      </x:c>
+      <x:c r="AE24" s="52" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="AF24" s="52">
+        <x:f>AE24</x:f>
+      </x:c>
+      <x:c r="AG24" s="52">
+        <x:f>+AA24-AC24+AE24</x:f>
+      </x:c>
+      <x:c r="AH24" s="52">
+        <x:f>+AB24-AD24+AF24</x:f>
+      </x:c>
+      <x:c r="AI24" s="52" t="s"/>
+      <x:c r="AJ24" s="52" t="s"/>
+      <x:c r="AK24" s="52">
+        <x:f>+AI24+AJ24</x:f>
+      </x:c>
+      <x:c r="AL24" s="52">
+        <x:f>+AB24-AD24+AI24</x:f>
+      </x:c>
+      <x:c r="AM24" s="52">
+        <x:f>+AF24+AJ24</x:f>
+      </x:c>
+      <x:c r="AN24" s="52">
+        <x:f>+AL24+AM24</x:f>
+      </x:c>
+      <x:c r="AO24" s="27" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="AP24" s="27" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="AV24" s="27" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="AW24" s="27" t="s"/>
+    </x:row>
+    <x:row r="25" spans="1:56">
+      <x:c r="Z25" s="53" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="AA25" s="53">
+        <x:f>SUM(AA10:AA24)</x:f>
+      </x:c>
+      <x:c r="AB25" s="53">
+        <x:f>SUM(AB10:AB24)</x:f>
+      </x:c>
+      <x:c r="AC25" s="53">
+        <x:f>SUM(AC10:AC24)</x:f>
+      </x:c>
+      <x:c r="AD25" s="53">
+        <x:f>SUM(AD10:AD24)</x:f>
+      </x:c>
+      <x:c r="AE25" s="53">
+        <x:f>SUM(AE10:AE24)</x:f>
+      </x:c>
+      <x:c r="AF25" s="53">
+        <x:f>SUM(AF10:AF24)</x:f>
+      </x:c>
+      <x:c r="AG25" s="53">
+        <x:f>SUM(AG10:AG24)</x:f>
+      </x:c>
+      <x:c r="AH25" s="53">
+        <x:f>SUM(AH10:AH24)</x:f>
+      </x:c>
+      <x:c r="AI25" s="53">
+        <x:f>SUM(AI10:AI24)</x:f>
+      </x:c>
+      <x:c r="AJ25" s="53">
+        <x:f>SUM(AJ10:AJ24)</x:f>
+      </x:c>
+      <x:c r="AK25" s="53">
+        <x:f>SUM(AK10:AK24)</x:f>
+      </x:c>
+      <x:c r="AL25" s="53">
+        <x:f>SUM(AL10:AL24)</x:f>
+      </x:c>
+      <x:c r="AM25" s="53">
+        <x:f>SUM(AM10:AM24)</x:f>
+      </x:c>
+      <x:c r="AN25" s="53">
+        <x:f>SUM(AN10:AN24)</x:f>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.19685039370078741" right="0.51181102362204722" top="0.984251968503937" bottom="0.984251968503937" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <x:pageSetup paperSize="8" scale="58" pageOrder="downThenOver" orientation="landscape" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="1" alignWithMargins="0">
+    <x:oddHeader/>
+    <x:oddFooter/>
+    <x:evenHeader/>
+    <x:evenFooter/>
+    <x:firstHeader/>
+    <x:firstFooter/>
+  </x:headerFooter>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>